<commit_message>
test passing on template_reader - single file
</commit_message>
<xml_diff>
--- a/tests/resources/test_template.xlsx
+++ b/tests/resources/test_template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -51,6 +51,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1837,7 +1838,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>